<commit_message>
NTC_calc. Add calculating for descrets
</commit_message>
<xml_diff>
--- a/NTC_calc.xlsx
+++ b/NTC_calc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Atmel-GlueGun\Atmel-GlueGun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Atmel-GlueGun\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>T0</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>R=</t>
+  </si>
+  <si>
+    <t>DR=</t>
+  </si>
+  <si>
+    <t>Rserial</t>
+  </si>
+  <si>
+    <t>Discr</t>
   </si>
 </sst>
 </file>
@@ -388,7 +397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -407,6 +418,12 @@
         <f>B1+273.15</f>
         <v>298.14999999999998</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -415,6 +432,12 @@
       <c r="B2">
         <v>3950</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>1023</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -427,7 +450,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="3">
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -454,11 +477,17 @@
       </c>
       <c r="E6" s="6">
         <f>POWER(EXP(1), $B$2*(1/($E$3+273.15) - 1/$C$1)+LN($B$4))</f>
-        <v>4070.8877664662809</v>
+        <v>1609.7003208467229</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="5"/>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5">
+        <f>1023-1023/$E$1*E6</f>
+        <v>858.32765717738027</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>

</xml_diff>